<commit_message>
Getting ready for internal reviewers.
</commit_message>
<xml_diff>
--- a/images/PSUTmats.xlsx
+++ b/images/PSUTmats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4B55D0-3262-4B4F-AA86-4B98E4E3AFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF5E6AF-A4D6-ED45-AF68-E59EDE618749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29280" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,12 +162,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD3712D"/>
+        <fgColor rgb="FFFDF2D0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFDF2D0"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -197,23 +198,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -514,7 +515,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -541,7 +542,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3"/>
@@ -550,19 +551,19 @@
         <v>0</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="9"/>
+      <c r="D3" s="8"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="9"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -574,17 +575,17 @@
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="7"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="4"/>

</xml_diff>